<commit_message>
corrected beamwidth for 18nm-S
</commit_message>
<xml_diff>
--- a/analysis/2019-06-12 results Wiener.xlsx
+++ b/analysis/2019-06-12 results Wiener.xlsx
@@ -5,19 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e453dee9ea284be0/PhD/DP-Experiment/analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Thomas\OneDrive\PhD\DP-Experiment\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="8_{3FCABA84-407A-425D-8891-B90CEA21B1B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{F7A4F8AA-03CC-417D-ABE3-054E4B0B757F}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="8_{3FCABA84-407A-425D-8891-B90CEA21B1B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{34FADE1D-510A-49D4-B497-9584951CF537}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="41280" windowHeight="27000" xr2:uid="{98E9D0D6-6A63-4C65-8D4C-4D11F684FB5E}"/>
   </bookViews>
   <sheets>
     <sheet name="Wiener-deconvolution_single_v2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -223,306 +220,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Chart1"/>
-      <sheetName val="Wiener-deconvolution_single_v2"/>
-      <sheetName val="Wiener-deconvolution_singleshot"/>
-      <sheetName val="Wiener_singleshot_xi_over_sig"/>
-      <sheetName val="Wiener_singleshot_zeta"/>
-      <sheetName val="Wiener-deconvolution_avg_image"/>
-      <sheetName val="Wiener_avg_image_xi_over_sig"/>
-      <sheetName val="Wiener-deconvolution_avg_im (2)"/>
-      <sheetName val="blind-deconvolution_avg_image"/>
-      <sheetName val="blind-deconv-xi_over_sig"/>
-      <sheetName val="blind-deconv_zeta"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="D2">
-            <v>0.30935251798561153</v>
-          </cell>
-          <cell r="M2">
-            <v>1.1797985611510793</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="D3">
-            <v>0.25353773584905659</v>
-          </cell>
-          <cell r="M3">
-            <v>1.1758018867924529</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="D4">
-            <v>1.2805755395683454</v>
-          </cell>
-          <cell r="M4">
-            <v>1.212705035971223</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="D5">
-            <v>1.0495283018867925</v>
-          </cell>
-          <cell r="M5">
-            <v>1.0878655660377359</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="D6">
-            <v>0.54568527918781728</v>
-          </cell>
-          <cell r="M6">
-            <v>1.891776649746193</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="D7">
-            <v>0.64759036144578308</v>
-          </cell>
-          <cell r="M7">
-            <v>2.4250602409638553</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="D8">
-            <v>0.81725888324873097</v>
-          </cell>
-          <cell r="M8">
-            <v>1.4645431472081218</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="D9">
-            <v>0.96987951807228912</v>
-          </cell>
-          <cell r="M9">
-            <v>2.0276506024096386</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="D10">
-            <v>1.1294416243654823</v>
-          </cell>
-          <cell r="M10">
-            <v>1.5842385786802031</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="D11">
-            <v>1.3403614457831325</v>
-          </cell>
-          <cell r="M11">
-            <v>2.5912951807228914</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="D12">
-            <v>1.7944162436548223</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="D13">
-            <v>2.1295180722891565</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="D14">
-            <v>0.57795698924731187</v>
-          </cell>
-          <cell r="M14">
-            <v>1.1381720430107527</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="D15">
-            <v>0.63421828908554567</v>
-          </cell>
-          <cell r="M15">
-            <v>1.7811799410029501</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="D16">
-            <v>0.86559139784946237</v>
-          </cell>
-          <cell r="M16">
-            <v>1.0250268817204302</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="D17">
-            <v>1.3648648648648649</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="D18">
-            <v>0.79527559055118113</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="D19">
-            <v>0.26161369193154033</v>
-          </cell>
-          <cell r="M19">
-            <v>1.5716625916870415</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="D20">
-            <v>1.0987654320987654</v>
-          </cell>
-          <cell r="M20">
-            <v>1.5422962962962963</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="E2">
-            <v>4.0215827338129499E-2</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="E3">
-            <v>1.0141509433962264E-2</v>
-          </cell>
-          <cell r="P3">
-            <v>8.4643396226415091E-2</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="E4">
-            <v>0.1664748201438849</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="E5">
-            <v>4.1981132075471703E-2</v>
-          </cell>
-          <cell r="P5">
-            <v>6.5034905660377368E-2</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="E6">
-            <v>1.6370558375634517E-2</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="E7">
-            <v>1.9427710843373493E-2</v>
-          </cell>
-          <cell r="P7">
-            <v>0.18464759036144579</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="E8">
-            <v>2.4517766497461929E-2</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="E9">
-            <v>2.9096385542168673E-2</v>
-          </cell>
-          <cell r="P9">
-            <v>0.16223132530120482</v>
-          </cell>
-        </row>
-        <row r="10">
-          <cell r="E10">
-            <v>3.3883248730964467E-2</v>
-          </cell>
-        </row>
-        <row r="11">
-          <cell r="E11">
-            <v>4.0210843373493975E-2</v>
-          </cell>
-          <cell r="P11">
-            <v>0.22393253012048192</v>
-          </cell>
-        </row>
-        <row r="12">
-          <cell r="E12">
-            <v>5.3832487309644669E-2</v>
-          </cell>
-        </row>
-        <row r="13">
-          <cell r="E13">
-            <v>6.3885542168674689E-2</v>
-          </cell>
-          <cell r="P13">
-            <v>0.22120843373493976</v>
-          </cell>
-        </row>
-        <row r="14">
-          <cell r="E14">
-            <v>1.7338709677419354E-2</v>
-          </cell>
-          <cell r="N14">
-            <v>0.17338709677419353</v>
-          </cell>
-        </row>
-        <row r="15">
-          <cell r="E15">
-            <v>1.9026548672566368E-2</v>
-          </cell>
-        </row>
-        <row r="16">
-          <cell r="E16">
-            <v>2.596774193548387E-2</v>
-          </cell>
-          <cell r="N16" t="e">
-            <v>#DIV/0!</v>
-          </cell>
-        </row>
-        <row r="17">
-          <cell r="E17">
-            <v>8.1891891891891888E-2</v>
-          </cell>
-          <cell r="N17">
-            <v>6.3011583011583008E-2</v>
-          </cell>
-        </row>
-        <row r="18">
-          <cell r="E18">
-            <v>3.1811023622047248E-2</v>
-          </cell>
-          <cell r="N18">
-            <v>2.6483689538807653E-2</v>
-          </cell>
-        </row>
-        <row r="19">
-          <cell r="E19">
-            <v>2.6161369193154035E-2</v>
-          </cell>
-          <cell r="N19">
-            <v>0.25666259168704153</v>
-          </cell>
-        </row>
-        <row r="20">
-          <cell r="E20">
-            <v>5.4938271604938277E-2</v>
-          </cell>
-          <cell r="N20">
-            <v>0.18853209876543212</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -825,7 +522,7 @@
   <dimension ref="A1:X21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,24 +876,24 @@
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>0.54568527918781728</v>
+        <v>0.49768518518518517</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" si="2"/>
-        <v>1.6370558375634517E-2</v>
+        <v>3.9814814814814817E-2</v>
       </c>
       <c r="G6" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="1">
-        <v>394</v>
+        <v>432</v>
       </c>
       <c r="I6" s="2">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="J6" s="5">
         <f t="shared" si="3"/>
-        <v>11.82</v>
+        <v>34.56</v>
       </c>
       <c r="K6" s="1">
         <v>745.36</v>
@@ -1210,20 +907,20 @@
       </c>
       <c r="N6" s="7">
         <f t="shared" si="1"/>
-        <v>1.891776649746193</v>
+        <v>1.7253703703703704</v>
       </c>
       <c r="O6" s="7"/>
       <c r="P6" s="6">
         <f t="shared" si="5"/>
-        <v>0.11300686916389395</v>
+        <v>0.16300686916389395</v>
       </c>
       <c r="Q6" s="8">
         <f t="shared" si="6"/>
-        <v>0.21378375634517766</v>
+        <v>0.2812472222222222</v>
       </c>
       <c r="R6">
         <f t="shared" si="7"/>
-        <v>1.2999868426735164</v>
+        <v>1.1270244334163626</v>
       </c>
       <c r="W6">
         <v>867.87</v>
@@ -1244,24 +941,24 @@
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>0.64759036144578308</v>
+        <v>0.56282722513089001</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="2"/>
-        <v>1.9427710843373493E-2</v>
+        <v>2.8141361256544501E-2</v>
       </c>
       <c r="G7" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="1">
-        <v>332</v>
+        <v>382</v>
       </c>
       <c r="I7" s="2">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="3"/>
-        <v>9.9599999999999991</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="K7" s="1">
         <v>805.12</v>
@@ -1275,20 +972,20 @@
       </c>
       <c r="N7" s="7">
         <f t="shared" si="1"/>
-        <v>2.4250602409638553</v>
+        <v>2.1076439790575918</v>
       </c>
       <c r="O7" s="7"/>
       <c r="P7" s="6">
         <f t="shared" si="5"/>
-        <v>0.10188990461049285</v>
+        <v>0.12188990461049286</v>
       </c>
       <c r="Q7" s="8">
         <f t="shared" si="6"/>
-        <v>0.24708915662650605</v>
+        <v>0.25690052356020948</v>
       </c>
       <c r="R7">
         <f t="shared" si="7"/>
-        <v>1.8708821584225137</v>
+        <v>1.5288597038209091</v>
       </c>
       <c r="W7">
         <v>769.44</v>
@@ -1309,24 +1006,24 @@
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>0.81725888324873097</v>
+        <v>0.74537037037037035</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="2"/>
-        <v>2.4517766497461929E-2</v>
+        <v>5.962962962962963E-2</v>
       </c>
       <c r="G8" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="1">
-        <v>394</v>
+        <v>432</v>
       </c>
       <c r="I8" s="2">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="J8" s="5">
         <f t="shared" si="3"/>
-        <v>11.82</v>
+        <v>34.56</v>
       </c>
       <c r="K8" s="1">
         <v>577.03</v>
@@ -1340,20 +1037,20 @@
       </c>
       <c r="N8" s="7">
         <f t="shared" si="1"/>
-        <v>1.4645431472081218</v>
+        <v>1.3357175925925926</v>
       </c>
       <c r="O8" s="7"/>
       <c r="P8" s="6">
         <f t="shared" si="5"/>
-        <v>0.13595636275410292</v>
+        <v>0.18595636275410293</v>
       </c>
       <c r="Q8" s="8">
         <f t="shared" si="6"/>
-        <v>0.19911395939086296</v>
+        <v>0.24838518518518521</v>
       </c>
       <c r="R8">
         <f t="shared" si="7"/>
-        <v>0.86526154897128793</v>
+        <v>0.74183930212323579</v>
       </c>
       <c r="W8">
         <v>566.59</v>
@@ -1374,24 +1071,24 @@
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>0.96987951807228912</v>
+        <v>0.84293193717277481</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="2"/>
-        <v>2.9096385542168673E-2</v>
+        <v>4.2146596858638745E-2</v>
       </c>
       <c r="G9" t="s">
         <v>14</v>
       </c>
       <c r="H9" s="1">
-        <v>332</v>
+        <v>382</v>
       </c>
       <c r="I9" s="2">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="3"/>
-        <v>9.9599999999999991</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="K9" s="1">
         <v>673.18</v>
@@ -1405,20 +1102,20 @@
       </c>
       <c r="N9" s="7">
         <f t="shared" si="1"/>
-        <v>2.0276506024096386</v>
+        <v>1.7622513089005234</v>
       </c>
       <c r="O9" s="7"/>
       <c r="P9" s="6">
         <f t="shared" si="5"/>
-        <v>0.10702249027006151</v>
+        <v>0.12702249027006152</v>
       </c>
       <c r="Q9" s="8">
         <f t="shared" si="6"/>
-        <v>0.2170042168674699</v>
+        <v>0.22384554973821991</v>
       </c>
       <c r="R9">
         <f t="shared" si="7"/>
-        <v>1.4435745508908391</v>
+        <v>1.1650309283306741</v>
       </c>
       <c r="W9">
         <v>546.67999999999995</v>
@@ -1439,24 +1136,24 @@
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>1.1294416243654823</v>
+        <v>1.0300925925925926</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="2"/>
-        <v>3.3883248730964467E-2</v>
+        <v>8.2407407407407401E-2</v>
       </c>
       <c r="G10" t="s">
         <v>13</v>
       </c>
       <c r="H10" s="1">
-        <v>394</v>
+        <v>432</v>
       </c>
       <c r="I10" s="2">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="J10" s="5">
         <f t="shared" si="3"/>
-        <v>11.82</v>
+        <v>34.56</v>
       </c>
       <c r="K10" s="1">
         <v>624.19000000000005</v>
@@ -1470,20 +1167,20 @@
       </c>
       <c r="N10" s="7">
         <f t="shared" si="1"/>
-        <v>1.5842385786802031</v>
+        <v>1.4448842592592595</v>
       </c>
       <c r="O10" s="7"/>
       <c r="P10" s="6">
         <f t="shared" si="5"/>
-        <v>0.14196911196911194</v>
+        <v>0.19196911196911196</v>
       </c>
       <c r="Q10" s="8">
         <f t="shared" si="6"/>
-        <v>0.22491294416243651</v>
+        <v>0.27737314814814817</v>
       </c>
       <c r="R10">
         <f t="shared" si="7"/>
-        <v>0.98368704215751934</v>
+        <v>0.84613534430673565</v>
       </c>
       <c r="W10">
         <v>573.69000000000005</v>
@@ -1504,24 +1201,24 @@
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>1.3403614457831325</v>
+        <v>1.1649214659685865</v>
       </c>
       <c r="F11" s="4">
         <f t="shared" si="2"/>
-        <v>4.0210843373493975E-2</v>
+        <v>5.8246073298429325E-2</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
       </c>
       <c r="H11" s="1">
-        <v>332</v>
+        <v>382</v>
       </c>
       <c r="I11" s="2">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="3"/>
-        <v>9.9599999999999991</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="K11" s="1">
         <v>860.31</v>
@@ -1535,20 +1232,20 @@
       </c>
       <c r="N11" s="7">
         <f t="shared" si="1"/>
-        <v>2.5912951807228914</v>
+        <v>2.2521204188481674</v>
       </c>
       <c r="O11" s="7"/>
       <c r="P11" s="6">
         <f t="shared" si="5"/>
-        <v>0.11549243877207054</v>
+        <v>0.13549243877207054</v>
       </c>
       <c r="Q11" s="8">
         <f t="shared" si="6"/>
-        <v>0.29927500000000001</v>
+        <v>0.30514528795811519</v>
       </c>
       <c r="R11">
         <f t="shared" si="7"/>
-        <v>2.0513583005689942</v>
+        <v>1.6839554015896081</v>
       </c>
       <c r="W11">
         <v>741.61</v>
@@ -1569,24 +1266,24 @@
       </c>
       <c r="E12" s="4">
         <f t="shared" si="0"/>
-        <v>1.7944162436548223</v>
+        <v>1.6365740740740742</v>
       </c>
       <c r="F12" s="4">
         <f t="shared" si="2"/>
-        <v>5.3832487309644669E-2</v>
+        <v>0.13092592592592595</v>
       </c>
       <c r="G12" t="s">
         <v>13</v>
       </c>
       <c r="H12" s="1">
-        <v>394</v>
+        <v>432</v>
       </c>
       <c r="I12" s="2">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="J12" s="5">
         <f t="shared" si="3"/>
-        <v>11.82</v>
+        <v>34.56</v>
       </c>
       <c r="M12" s="6"/>
       <c r="N12" s="7"/>
@@ -1609,24 +1306,24 @@
       </c>
       <c r="E13" s="4">
         <f t="shared" si="0"/>
-        <v>2.1295180722891565</v>
+        <v>1.8507853403141361</v>
       </c>
       <c r="F13" s="4">
         <f t="shared" si="2"/>
-        <v>6.3885542168674689E-2</v>
+        <v>9.2539267015706805E-2</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="1">
-        <v>332</v>
+        <v>382</v>
       </c>
       <c r="I13" s="2">
-        <v>0.03</v>
+        <v>0.05</v>
       </c>
       <c r="J13" s="5">
         <f t="shared" si="3"/>
-        <v>9.9599999999999991</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="M13" s="6"/>
       <c r="N13" s="7"/>

</xml_diff>